<commit_message>
Utilizing add data element in queue and process on application
</commit_message>
<xml_diff>
--- a/InvokeWorkFlow/InvokeWorkflow.xlsx
+++ b/InvokeWorkFlow/InvokeWorkflow.xlsx
@@ -97,13 +97,13 @@
   </x:cellStyleXfs>
   <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -429,7 +429,7 @@
   <x:dimension ref="A1:F4"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="H4" sqref="H4 H4:H4"/>
+      <x:selection activeCell="F4" sqref="F4 F4:F4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
     <x:col min="6" max="6" width="15.285156" style="5" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -462,7 +462,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="5" t="n">
         <x:v>25</x:v>
       </x:c>
@@ -482,7 +482,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="5" t="n">
         <x:v>40</x:v>
       </x:c>
@@ -502,7 +502,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="5" t="n">
         <x:v>15</x:v>
       </x:c>

</xml_diff>